<commit_message>
extra waarden als resultaten
</commit_message>
<xml_diff>
--- a/meting WV py test.xlsx
+++ b/meting WV py test.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -448,520 +448,545 @@
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
           <t>EU</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="0" t="inlineStr">
         <is>
           <t>OM</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="0" t="inlineStr">
         <is>
           <t>AX</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="0" t="inlineStr">
         <is>
           <t>HO</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="0" t="inlineStr">
         <is>
           <t>RO</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="0" t="inlineStr">
         <is>
           <t>n</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="0" t="inlineStr">
         <is>
           <t>all times are in ms</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>0.07197642000000393</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0.058047280000010915</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.14118679999997497</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0.38524693999997695</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0.4317532000000224</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>4520.739832</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>3396.5556349999993</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>7364.308857999999</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>16783.801179</t>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t>22977.184621999997</t>
+        </is>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>0.23617237999997265</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>0.1147442799999876</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.3398531800000537</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0.7045062600000485</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0.9717117200000303</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>8674.385119999997</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>6575.919615000003</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>14572.916676999996</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>33520.63456499999</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>46143.18019299999</t>
+        </is>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>0.37178304000001994</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>0.26274395999998923</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.5832295000000087</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1.2070546599999954</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1.6362909199999542</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>17505.421296999997</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>13122.930255999989</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>29212.589455</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>66916.72769099998</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>92091.07091100003</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>0.7125132800000333</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0.5322533600000057</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1.1042078599999972</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2.3149235999999807</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>3.1754439999999917</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>34993.51118099997</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>26284.58743699997</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>58428.931455</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>134900.58596100003</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>184947.50486099996</t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1.2757005799999988</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1.0188896000000014</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2.002476660000001</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>4.551924679999955</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>6.2373429999999885</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>70649.45734499997</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>52244.13258100003</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>117184.53777700006</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>268124.09309700003</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>367320.8603580001</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2.3868115199999984</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1.894817760000027</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>3.9483152200000764</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>8.788910859999959</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>12.182545139999945</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>155505.491163</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>116712.30815800004</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>246883.17314300002</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>577086.9314040001</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>795402.6730360001</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="0" t="inlineStr">
         <is>
           <t>4.54004604000005</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>3.564782939999933</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="0" t="inlineStr">
         <is>
           <t>7.750753879999994</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="0" t="inlineStr">
         <is>
           <t>17.457643460000103</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="0" t="inlineStr">
         <is>
           <t>23.601877060000014</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="F8" s="0" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="0" t="inlineStr">
         <is>
           <t>9.113197939999935</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>6.91619253999999</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="0" t="inlineStr">
         <is>
           <t>14.691266680000012</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="0" t="inlineStr">
         <is>
           <t>33.77649181999999</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="0" t="inlineStr">
         <is>
           <t>48.194687700000145</t>
         </is>
       </c>
-      <c r="F9" t="n">
+      <c r="F9" s="0" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="0" t="inlineStr">
         <is>
           <t>17.535119100000216</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>13.80839765999994</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="0" t="inlineStr">
         <is>
           <t>30.170136840000197</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="0" t="inlineStr">
         <is>
           <t>71.34628643999996</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="0" t="inlineStr">
         <is>
           <t>97.08236501999991</t>
         </is>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" s="0" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="0" t="inlineStr">
         <is>
           <t>35.91034019999981</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr">
         <is>
           <t>28.331284400000243</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="0" t="inlineStr">
         <is>
           <t>61.331507720000005</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>138.63258150000064</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="0" t="inlineStr">
         <is>
           <t>185.4951604599998</t>
         </is>
       </c>
-      <c r="F11" t="n">
+      <c r="F11" s="0" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="0" t="inlineStr">
         <is>
           <t>71.59075429999973</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>57.41797394000031</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="0" t="inlineStr">
         <is>
           <t>120.56409872000032</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="0" t="inlineStr">
         <is>
           <t>323.6806076999994</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" s="0" t="inlineStr">
         <is>
           <t>407.1781429400019</t>
         </is>
       </c>
-      <c r="F12" t="n">
+      <c r="F12" s="0" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="0" t="inlineStr">
         <is>
           <t>161.46866857999896</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
         <is>
           <t>119.79441692000051</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>295.02627080000025</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="0" t="inlineStr">
         <is>
           <t>689.0536485999991</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" s="0" t="inlineStr">
         <is>
           <t>867.1011679800006</t>
         </is>
       </c>
-      <c r="F13" t="n">
+      <c r="F13" s="0" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="0" t="inlineStr">
         <is>
           <t>311.1845970600018</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
         <is>
           <t>237.5737131400001</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>513.7195911999987</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="0" t="inlineStr">
         <is>
           <t>1154.785946620002</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" s="0" t="inlineStr">
         <is>
           <t>1542.943631959996</t>
         </is>
       </c>
-      <c r="F14" t="n">
+      <c r="F14" s="0" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="0" t="inlineStr">
         <is>
           <t>586.840522699996</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
         <is>
           <t>443.7957570600031</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>1021.4612049600009</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="0" t="inlineStr">
         <is>
           <t>2417.125553420007</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" s="0" t="inlineStr">
         <is>
           <t>3024.6701319000044</t>
         </is>
       </c>
-      <c r="F15" t="n">
+      <c r="F15" s="0" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="0" t="inlineStr">
         <is>
           <t>1098.102418939991</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>871.5627096400021</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>1874.610400620004</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>4430.2807691800035</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E16" s="0" t="inlineStr">
         <is>
           <t>6618.059418019984</t>
         </is>
       </c>
-      <c r="F16" t="n">
+      <c r="F16" s="0" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="0" t="inlineStr">
         <is>
           <t>2505.087953819989</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>1990.2620206999973</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>4329.864055280009</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="0" t="inlineStr">
         <is>
           <t>9226.05444593999</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E17" s="0" t="inlineStr">
         <is>
           <t>12801.402118179994</t>
         </is>
       </c>
-      <c r="F17" t="n">
-        <v>16</v>
+      <c r="F17" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="F18" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="F19" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="F20" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="F21" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="F22" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>